<commit_message>
change in storage "power_tri" matrix & new folder
Matrice power_tri ora a blocchi.
Nuovi grafici di risultati
</commit_message>
<xml_diff>
--- a/tesi_camilla/case1_home/Concettuale_caso1_casa.xlsx
+++ b/tesi_camilla/case1_home/Concettuale_caso1_casa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cami/Documents/GitHub/pyesm_thesis/tesi_camilla/case1_home/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45962381-73AC-B64D-96AC-12832B2618EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21C6647-8FA0-3748-B379-747C5537FB32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-780" yWindow="-17500" windowWidth="32000" windowHeight="17500" xr2:uid="{7B02621E-B7BE-C640-8F0D-21B2A43A72CA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{7B02621E-B7BE-C640-8F0D-21B2A43A72CA}"/>
   </bookViews>
   <sheets>
     <sheet name="new_limit" sheetId="23" r:id="rId1"/>
@@ -1059,7 +1059,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.00;\-#,##0.00;\-"/>
     <numFmt numFmtId="167" formatCode="#,##0.00000;\-#,##0.00000;\-"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1153,12 +1153,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow (Body)"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="17">
@@ -1838,11 +1832,11 @@
   <dimension ref="A1:CN96"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F6" zoomScale="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="BU48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="AK26" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F6" sqref="F6"/>
       <selection pane="topRight" activeCell="I6" sqref="I6"/>
       <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
-      <selection pane="bottomRight" activeCell="CB67" sqref="CB67"/>
+      <selection pane="bottomRight" activeCell="AO36" sqref="AO36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5985,22 +5979,22 @@
       <c r="BR29" s="6"/>
       <c r="BZ29" s="13"/>
       <c r="CA29" s="20">
-        <v>184.6</v>
+        <v>164.7</v>
       </c>
       <c r="CB29" s="13">
-        <v>199</v>
+        <v>179.1</v>
       </c>
       <c r="CC29" s="13">
-        <v>184.6</v>
+        <v>164.7</v>
       </c>
       <c r="CD29" s="13">
-        <v>181.16</v>
+        <v>161.26</v>
       </c>
       <c r="CE29" s="13">
-        <v>181.16</v>
+        <v>161.26</v>
       </c>
       <c r="CF29" s="21">
-        <v>190.36</v>
+        <v>170.45999999999998</v>
       </c>
       <c r="CG29">
         <v>0</v>
@@ -7030,7 +7024,7 @@
         <v>60</v>
       </c>
       <c r="AU39" s="16">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="AV39" s="16">
         <v>160</v>
@@ -8154,7 +8148,7 @@
       <c r="AW49" s="13"/>
       <c r="AX49" s="42" cm="1">
         <f t="array" ref="AX49:AX54">BB57:BB62-MMULT(BH41:BM46,MMULT(S49:AI54,BL19:BL35))</f>
-        <v>39.1</v>
+        <v>34.1</v>
       </c>
       <c r="AY49" s="13"/>
       <c r="AZ49" s="48">
@@ -8312,7 +8306,7 @@
       </c>
       <c r="AW50" s="13"/>
       <c r="AX50" s="43">
-        <v>39.1</v>
+        <v>34.1</v>
       </c>
       <c r="AY50" s="13"/>
       <c r="AZ50" s="48">
@@ -8485,7 +8479,7 @@
       </c>
       <c r="AW51" s="13"/>
       <c r="AX51" s="43">
-        <v>28.2</v>
+        <v>23.2</v>
       </c>
       <c r="AY51" s="13"/>
       <c r="AZ51" s="48">
@@ -8653,7 +8647,7 @@
       </c>
       <c r="AW52" s="13"/>
       <c r="AX52" s="43">
-        <v>27.979999999999997</v>
+        <v>22.979999999999997</v>
       </c>
       <c r="AY52" s="13"/>
       <c r="AZ52" s="48">
@@ -8803,7 +8797,7 @@
       </c>
       <c r="AW53" s="13"/>
       <c r="AX53" s="43">
-        <v>10.14</v>
+        <v>5.1400000000000006</v>
       </c>
       <c r="AY53" s="13"/>
       <c r="AZ53" s="48">
@@ -8845,22 +8839,22 @@
       <c r="BZ53" s="13"/>
       <c r="CA53" cm="1">
         <f t="array" ref="CA53:CF53">TRANSPOSE(BA57:BA62-_xlfn.ANCHORARRAY(AX49))</f>
-        <v>59.9</v>
+        <v>54.999999999999993</v>
       </c>
       <c r="CB53">
-        <v>59.9</v>
+        <v>54.999999999999993</v>
       </c>
       <c r="CC53">
-        <v>70.8</v>
+        <v>65.899999999999991</v>
       </c>
       <c r="CD53">
-        <v>71.02000000000001</v>
+        <v>66.12</v>
       </c>
       <c r="CE53">
-        <v>88.86</v>
+        <v>83.96</v>
       </c>
       <c r="CF53">
-        <v>94</v>
+        <v>89.1</v>
       </c>
     </row>
     <row r="54" spans="1:92" x14ac:dyDescent="0.2">
@@ -8970,7 +8964,7 @@
       </c>
       <c r="AW54" s="13"/>
       <c r="AX54" s="43">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AY54" s="13"/>
       <c r="AZ54" s="48">
@@ -9105,22 +9099,22 @@
       <c r="BZ55" s="13"/>
       <c r="CA55" s="36" cm="1">
         <f t="array" ref="CA55:CF55">TRANSPOSE(_xlfn.ANCHORARRAY(AX49)-AZ57:AZ62)</f>
-        <v>34.1</v>
+        <v>29.6</v>
       </c>
       <c r="CB55">
-        <v>34.1</v>
+        <v>29.6</v>
       </c>
       <c r="CC55">
-        <v>23.2</v>
+        <v>18.7</v>
       </c>
       <c r="CD55">
-        <v>22.979999999999997</v>
+        <v>18.479999999999997</v>
       </c>
       <c r="CE55">
-        <v>5.1400000000000006</v>
+        <v>0.64000000000000057</v>
       </c>
       <c r="CF55">
-        <v>0</v>
+        <v>-4.5</v>
       </c>
     </row>
     <row r="56" spans="1:92" x14ac:dyDescent="0.2">
@@ -9267,13 +9261,13 @@
       </c>
       <c r="AZ57" s="33" cm="1">
         <f t="array" ref="AZ57:BB62">AZ49:BB54*AU87</f>
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="BA57" s="33">
-        <v>99</v>
+        <v>89.1</v>
       </c>
       <c r="BB57" s="33">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="CA57" s="11" t="s">
         <v>150</v>
@@ -9368,13 +9362,13 @@
         <v>-5.5733333333333341</v>
       </c>
       <c r="AZ58" s="33">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="BA58" s="33">
-        <v>99</v>
+        <v>89.1</v>
       </c>
       <c r="BB58" s="33">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="BK58" s="13"/>
       <c r="BL58" s="13"/>
@@ -9490,13 +9484,13 @@
         <v>-5.5733333333333341</v>
       </c>
       <c r="AZ59" s="33">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="BA59" s="33">
-        <v>99</v>
+        <v>89.1</v>
       </c>
       <c r="BB59" s="33">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="BL59" s="13"/>
       <c r="CA59">
@@ -9610,13 +9604,13 @@
         <v>-5.5733333333333341</v>
       </c>
       <c r="AZ60" s="33">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="BA60" s="33">
-        <v>99</v>
+        <v>89.1</v>
       </c>
       <c r="BB60" s="33">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="BL60" s="13"/>
     </row>
@@ -9720,13 +9714,13 @@
         <v>-5.5733333333333341</v>
       </c>
       <c r="AZ61" s="33">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="BA61" s="33">
-        <v>99</v>
+        <v>89.1</v>
       </c>
       <c r="BB61" s="33">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="BL61" s="13"/>
       <c r="CA61" t="s">
@@ -9846,13 +9840,13 @@
       <c r="AW62" s="13"/>
       <c r="AX62" s="13"/>
       <c r="AZ62" s="33">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="BA62" s="33">
-        <v>99</v>
+        <v>89.1</v>
       </c>
       <c r="BB62" s="33">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="BL62" s="13"/>
       <c r="BZ62" s="13" t="s">
@@ -9890,7 +9884,7 @@
         <v>-60</v>
       </c>
       <c r="CK62">
-        <v>-100</v>
+        <v>-90</v>
       </c>
       <c r="CL62">
         <v>-160</v>
@@ -10033,7 +10027,7 @@
         <v>60</v>
       </c>
       <c r="CK63">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="CL63">
         <v>160</v>
@@ -10113,7 +10107,7 @@
         <v>60</v>
       </c>
       <c r="AU65" s="34">
-        <v>199</v>
+        <v>179.1</v>
       </c>
       <c r="AV65" s="34">
         <v>160</v>
@@ -10186,7 +10180,7 @@
         <v>60</v>
       </c>
       <c r="AU66" s="34">
-        <v>199</v>
+        <v>179.1</v>
       </c>
       <c r="AV66" s="34">
         <v>160</v>
@@ -10267,7 +10261,7 @@
         <v>60</v>
       </c>
       <c r="AU67" s="34">
-        <v>199</v>
+        <v>179.1</v>
       </c>
       <c r="AV67" s="34">
         <v>160</v>
@@ -10342,7 +10336,7 @@
         <v>60</v>
       </c>
       <c r="AU68" s="34">
-        <v>199</v>
+        <v>179.1</v>
       </c>
       <c r="AV68" s="34">
         <v>160</v>
@@ -10416,7 +10410,7 @@
         <v>60</v>
       </c>
       <c r="AU69" s="34">
-        <v>199</v>
+        <v>179.1</v>
       </c>
       <c r="AV69" s="34">
         <v>160</v>
@@ -10496,7 +10490,7 @@
         <v>60</v>
       </c>
       <c r="AU70" s="34">
-        <v>199</v>
+        <v>179.1</v>
       </c>
       <c r="AV70" s="34">
         <v>160</v>
@@ -11206,7 +11200,7 @@
       </c>
       <c r="I81" s="3"/>
       <c r="J81" s="3">
-        <f>1/(1+$J$16)^H81</f>
+        <f t="shared" ref="J81:J90" si="0">1/(1+$J$16)^H81</f>
         <v>1</v>
       </c>
       <c r="K81" s="3"/>
@@ -11273,7 +11267,7 @@
       </c>
       <c r="I82" s="3"/>
       <c r="J82" s="3">
-        <f>1/(1+$J$16)^H82</f>
+        <f t="shared" si="0"/>
         <v>0.95923261390887293</v>
       </c>
       <c r="K82" s="3"/>
@@ -11301,7 +11295,7 @@
       </c>
       <c r="I83" s="3"/>
       <c r="J83" s="3">
-        <f>1/(1+$J$16)^H83</f>
+        <f t="shared" si="0"/>
         <v>0.92012720758644884</v>
       </c>
       <c r="K83" s="3"/>
@@ -11365,7 +11359,7 @@
       </c>
       <c r="I84" s="3"/>
       <c r="J84" s="3">
-        <f>1/(1+$J$16)^H84</f>
+        <f t="shared" si="0"/>
         <v>0.88261602646182147</v>
       </c>
       <c r="K84" s="3"/>
@@ -11393,7 +11387,7 @@
       </c>
       <c r="I85" s="3"/>
       <c r="J85" s="3">
-        <f>1/(1+$J$16)^H85</f>
+        <f t="shared" si="0"/>
         <v>0.84663407814083602</v>
       </c>
       <c r="K85" s="3"/>
@@ -11461,7 +11455,7 @@
       </c>
       <c r="I86" s="3"/>
       <c r="J86" s="3">
-        <f>1/(1+$J$16)^H86</f>
+        <f t="shared" si="0"/>
         <v>0.81211901979936307</v>
       </c>
       <c r="K86" s="3"/>
@@ -11492,7 +11486,7 @@
       </c>
       <c r="I87" s="3"/>
       <c r="J87" s="3">
-        <f>1/(1+$J$16)^H87</f>
+        <f t="shared" si="0"/>
         <v>0.7790110501672548</v>
       </c>
       <c r="K87" s="3"/>
@@ -11547,7 +11541,7 @@
         <v>82</v>
       </c>
       <c r="AG87" s="34">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="AH87" s="34">
         <v>160</v>
@@ -11587,7 +11581,7 @@
         <v>60</v>
       </c>
       <c r="AU87" s="35">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="AV87" s="35">
         <v>160</v>
@@ -11612,7 +11606,7 @@
       </c>
       <c r="I88" s="3"/>
       <c r="J88" s="3">
-        <f>1/(1+$J$16)^H88</f>
+        <f t="shared" si="0"/>
         <v>0.74725280591583187</v>
       </c>
       <c r="K88" s="3"/>
@@ -11640,7 +11634,7 @@
       </c>
       <c r="I89" s="3"/>
       <c r="J89" s="3">
-        <f>1/(1+$J$16)^H89</f>
+        <f t="shared" si="0"/>
         <v>0.71678926226938311</v>
       </c>
       <c r="K89" s="3"/>
@@ -11707,7 +11701,7 @@
       </c>
       <c r="I90" s="3"/>
       <c r="J90" s="3">
-        <f>1/(1+$J$16)^H90</f>
+        <f t="shared" si="0"/>
         <v>0.68756763766847306</v>
       </c>
       <c r="K90" s="3"/>

</xml_diff>